<commit_message>
empty files bug fix
</commit_message>
<xml_diff>
--- a/test/testETN.xlsx
+++ b/test/testETN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_server\EasyTranslations\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2DACAA-6585-4515-B052-C086D27FCC97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5A5A28-B05C-4FDC-A008-747D5A1F4CD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>title</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Welcome</t>
+  </si>
+  <si>
+    <t>domain</t>
   </si>
 </sst>
 </file>
@@ -418,19 +421,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.375" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -442,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -456,7 +457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -467,7 +468,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -481,144 +482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="130" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="132" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="137" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="3:4" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
     </row>

</xml_diff>